<commit_message>
Finishing up Quadrupole technote
</commit_message>
<xml_diff>
--- a/quads/Patsy2012.xlsx
+++ b/quads/Patsy2012.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="460" windowWidth="26920" windowHeight="16260"/>
+    <workbookView xWindow="4680" yWindow="1540" windowWidth="26920" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>BL</t>
   </si>
@@ -110,6 +110,31 @@
   <si>
     <t>Old Map 
 GL (G)</t>
+  </si>
+  <si>
+    <t>Residual Param</t>
+  </si>
+  <si>
+    <t>Residual G4 Param</t>
+  </si>
+  <si>
+    <t>UK Meas</t>
+  </si>
+  <si>
+    <t>Curr/300A</t>
+  </si>
+  <si>
+    <t>DIffx100 (T)</t>
+  </si>
+  <si>
+    <t>Diff(%)</t>
+  </si>
+  <si>
+    <t>Measured
+GL (T)</t>
+  </si>
+  <si>
+    <t>Diff(%) UK-LANL</t>
   </si>
 </sst>
 </file>
@@ -881,7 +906,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -889,7 +914,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Measured GL vs Current (2012 Measurement)</a:t>
             </a:r>
           </a:p>
@@ -899,7 +928,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2104871121879"/>
+          <c:x val="0.270316172016959"/>
           <c:y val="0.0286458333333333"/>
         </c:manualLayout>
       </c:layout>
@@ -918,7 +947,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -931,7 +960,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0888575274244565"/>
+          <c:y val="0.107005208333333"/>
+          <c:w val="0.82669089440743"/>
+          <c:h val="0.66980561023622"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -986,29 +1025,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent1"/>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1000"/>
-                      <a:t>y = 0.2121x5 + 0.0318x4 - 0.1038x3 - 0.0135x2 - 5.3544x - 0.0234</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00779016084527892"/>
+                  <c:y val="0.564869791666667"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:solidFill>
@@ -1024,9 +1046,11 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent1"/>
+                        <a:schemeClr val="accent5">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -1096,52 +1120,66 @@
                 <c:formatCode>0.0000000</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-5.232144</c:v>
+                  <c:v>5.232144</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.446660457142858</c:v>
+                  <c:v>4.446660457142858</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.581072628571428</c:v>
+                  <c:v>3.581072628571428</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.698637828571428</c:v>
+                  <c:v>2.698637828571428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.813790085714286</c:v>
+                  <c:v>1.813790085714286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.9236994</c:v>
+                  <c:v>0.9236994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.211979114285714</c:v>
+                  <c:v>0.211979114285714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.164829171428571</c:v>
+                  <c:v>-0.164829171428571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8755328</c:v>
+                  <c:v>-0.8755328</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.764304142857143</c:v>
+                  <c:v>-1.764304142857143</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.648062571428571</c:v>
+                  <c:v>-2.648062571428571</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.529865571428571</c:v>
+                  <c:v>-3.529865571428571</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.394514114285713</c:v>
+                  <c:v>-4.394514114285713</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.227943685714285</c:v>
+                  <c:v>-5.227943685714285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1523489008"/>
+        <c:axId val="-1495687312"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="6"/>
           <c:order val="1"/>
@@ -1239,43 +1277,43 @@
                   <c:v>-0.0528807353221707</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.183805272723786</c:v>
+                  <c:v>0.18500011727223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.124492183251713</c:v>
+                  <c:v>-0.122804213489848</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.163427600700409</c:v>
+                  <c:v>-0.161218893862833</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0615002704309716</c:v>
+                  <c:v>0.0645238686694655</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.271054386398584</c:v>
+                  <c:v>0.276311471105161</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.810375818243113</c:v>
+                  <c:v>0.830820739857667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.640888137451658</c:v>
+                  <c:v>0.616203589304855</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0612428692865827</c:v>
+                  <c:v>0.0571157653204654</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0468039419625223</c:v>
+                  <c:v>-0.0486328087318383</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.185118989596552</c:v>
+                  <c:v>-0.186350137082905</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.449385915813744</c:v>
+                  <c:v>0.44823076024032</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.315302145696912</c:v>
+                  <c:v>-0.31677480492965</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0759376038728131</c:v>
+                  <c:v>0.0737838988998947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,8 +1348,8 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -1430,161 +1468,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1523489008"/>
-        <c:axId val="-1495687312"/>
-      </c:scatterChart>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Fit Residual (%)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Summary!$U$3:$U$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000000</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.99639</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.830173333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.664753333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.499003333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.333396666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.167513333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0348866666666667</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.0349666666666667</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.167773333333333</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.333686666666667</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.498926666666667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.66002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.83119</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.99641</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Summary!$W$3:$W$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>-0.0528807353221707</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.183805272723786</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.124492183251713</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.163427600700409</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0615002704309716</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.271054386398584</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.810375818243113</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.640888137451658</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0612428692865827</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.0468039419625223</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.185118989596552</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.449385915813744</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.315302145696912</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0759376038728131</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-1523489008"/>
-        <c:axId val="-1495687312"/>
+        <c:axId val="-1477623968"/>
+        <c:axId val="-1526684528"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="-1523489008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+          <c:min val="-1.2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1609,9 +1501,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1619,7 +1511,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Current/300 A</a:t>
                 </a:r>
               </a:p>
@@ -1629,8 +1525,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.363469950871526"/>
-              <c:y val="0.944760498687664"/>
+              <c:x val="0.443811831213406"/>
+              <c:y val="0.835385498687664"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1646,9 +1542,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="accent1"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1681,9 +1577,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1696,6 +1592,7 @@
         <c:crossAx val="-1495687312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="-1495687312"/>
@@ -1725,6 +1622,121 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>GL (T)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0188767750185073"/>
+              <c:y val="0.432035351049869"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1523489008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1526684528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.0"/>
+          <c:min val="-3.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="accent1"/>
@@ -1735,9 +1747,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Measured GL (T cm)</a:t>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Residual</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1745,8 +1774,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0171673819742489"/>
-              <c:y val="0.291410406469462"/>
+              <c:x val="0.961282051282051"/>
+              <c:y val="0.359329888451443"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1775,10 +1804,9 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
+        <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1797,9 +1825,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1809,8 +1837,21 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1523489008"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="-1477623968"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1477623968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1526684528"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1822,39 +1863,19 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:legendEntry>
         <c:idx val="3"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.801655831482603"/>
-          <c:y val="0.287453248031496"/>
-          <c:w val="0.198344168517397"/>
-          <c:h val="0.466219408384763"/>
+          <c:x val="0.0722701393095094"/>
+          <c:y val="0.909918389107612"/>
+          <c:w val="0.877681943603203"/>
+          <c:h val="0.0900816108923884"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1870,9 +1891,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2036,7 +2057,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Difference x100 (T)</c:v>
           </c:tx>
@@ -2138,72 +2159,72 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AB$3:$AB$23</c:f>
+              <c:f>Summary!$AA$3:$AA$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3.465499999999988</c:v>
+                  <c:v>-3.465499999999988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.992029100000071</c:v>
+                  <c:v>-2.992029100000071</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.807539199999987</c:v>
+                  <c:v>-2.807539199999987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.82045729999998</c:v>
+                  <c:v>-3.82045729999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.717262400000032</c:v>
+                  <c:v>-4.717262400000032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.883437500000021</c:v>
+                  <c:v>-4.883437500000021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.817421600000049</c:v>
+                  <c:v>-4.817421600000049</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.820861700000001</c:v>
+                  <c:v>-4.820861700000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.896864800000022</c:v>
+                  <c:v>-4.896864800000022</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.056049900000003</c:v>
+                  <c:v>-5.056049900000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.24</c:v>
+                  <c:v>-5.24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.532014099999992</c:v>
+                  <c:v>-4.532014099999992</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.339959200000009</c:v>
+                  <c:v>-3.339959200000009</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.35622230000001</c:v>
+                  <c:v>-2.35622230000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.261062400000013</c:v>
+                  <c:v>-1.261062400000013</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0789625000000349</c:v>
+                  <c:v>-0.0789625000000349</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-1.155918399999978</c:v>
+                  <c:v>1.155918399999978</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.232993299999952</c:v>
+                  <c:v>2.232993299999952</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.057595200000041</c:v>
+                  <c:v>3.057595200000041</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-4.949925100000118</c:v>
+                  <c:v>4.949925100000118</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-8.262300000000078</c:v>
+                  <c:v>8.262300000000078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2242,11 +2263,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2269,8 +2290,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0323483474927476"/>
-                  <c:y val="-0.534655149064598"/>
+                  <c:x val="0.0413204517198508"/>
+                  <c:y val="-0.106730639014104"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2279,7 +2300,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="tx1">
                             <a:lumMod val="65000"/>
@@ -2292,86 +2313,86 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>y = 0.2121x</a:t>
+                      <a:t>y = -0.2121x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="30000">
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>5</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t> + 0.0318x</a:t>
+                      <a:t> - 0.0318x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="30000">
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>4</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t> - 0.1038x</a:t>
+                      <a:t> + 0.1038x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="30000">
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>3</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t> - 0.0135x</a:t>
+                      <a:t> + 0.0135x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="30000">
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>2</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx2"/>
+                          <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t> - 5.3544x - 0.0234</a:t>
+                      <a:t> + 5.3544x + 0.0234</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="1100">
+                    <a:endParaRPr lang="en-US" sz="1200">
                       <a:solidFill>
-                        <a:schemeClr val="tx2"/>
+                        <a:schemeClr val="accent1"/>
                       </a:solidFill>
                     </a:endParaRPr>
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -2384,7 +2405,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -2459,46 +2480,46 @@
                 <c:formatCode>0.0000000</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>-5.232144</c:v>
+                  <c:v>5.232144</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.446660457142858</c:v>
+                  <c:v>4.446660457142858</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.581072628571428</c:v>
+                  <c:v>3.581072628571428</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.698637828571428</c:v>
+                  <c:v>2.698637828571428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.813790085714286</c:v>
+                  <c:v>1.813790085714286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.9236994</c:v>
+                  <c:v>0.9236994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.211979114285714</c:v>
+                  <c:v>0.211979114285714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.164829171428571</c:v>
+                  <c:v>-0.164829171428571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8755328</c:v>
+                  <c:v>-0.8755328</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.764304142857143</c:v>
+                  <c:v>-1.764304142857143</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.648062571428571</c:v>
+                  <c:v>-2.648062571428571</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.529865571428571</c:v>
+                  <c:v>-3.529865571428571</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.394514114285713</c:v>
+                  <c:v>-4.394514114285713</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.227943685714285</c:v>
+                  <c:v>-5.227943685714285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2539,9 +2560,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -2554,10 +2573,108 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0175428667633651"/>
-                  <c:y val="-0.492169320358297"/>
+                  <c:x val="0.0181843141317862"/>
+                  <c:y val="-0.0558503743543113"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>y = -0.2734x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>5</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> - 0.0516x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>4</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> + 0.163x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> + 0.1018x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="30000">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="7030A0"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> + 5.2999x - 0.023</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200">
+                      <a:solidFill>
+                        <a:srgbClr val="7030A0"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2571,10 +2688,11 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6">
-                          <a:lumMod val="50000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -2666,67 +2784,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-5.216545</c:v>
+                  <c:v>5.216545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.752937999999999</c:v>
+                  <c:v>4.752937999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.258104</c:v>
+                  <c:v>4.258104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.732211</c:v>
+                  <c:v>3.732211</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.195534</c:v>
+                  <c:v>3.195534</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.6595</c:v>
+                  <c:v>2.6595</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.122803</c:v>
+                  <c:v>2.122803</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.584756</c:v>
+                  <c:v>1.584756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.046563</c:v>
+                  <c:v>1.046563</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.508513</c:v>
+                  <c:v>0.508513</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.029</c:v>
+                  <c:v>-0.029</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55733</c:v>
+                  <c:v>-0.55733</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.081153</c:v>
+                  <c:v>-1.081153</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.607812</c:v>
+                  <c:v>-1.607812</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.134096</c:v>
+                  <c:v>-2.134096</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.659549</c:v>
+                  <c:v>-2.659549</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.18287</c:v>
+                  <c:v>-3.18287</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.703326</c:v>
+                  <c:v>-3.703326</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.217574</c:v>
+                  <c:v>-4.217574</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.706417</c:v>
+                  <c:v>-4.706417</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.158377</c:v>
+                  <c:v>-5.158377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2749,9 +2867,9 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Parametrization Difference (%)</c:v>
+            <c:v>Parametrization Diff (%)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2851,7 +2969,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AC$3:$AC$23</c:f>
+              <c:f>Summary!$AB$3:$AB$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2928,8 +3046,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1476505760"/>
-        <c:axId val="-1493707728"/>
+        <c:axId val="-1630977712"/>
+        <c:axId val="-1459349776"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="-1493616000"/>
@@ -3189,81 +3307,13 @@
         <c:majorUnit val="3.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1493707728"/>
+        <c:axId val="-1459349776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12.0"/>
-          <c:min val="-12.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Parametrization Diff (%)</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1200">
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3271,8 +3321,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="75000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -3286,8 +3337,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -3298,13 +3350,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1476505760"/>
+        <c:crossAx val="-1630977712"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1476505760"/>
+        <c:axId val="-1630977712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3313,7 +3365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1493707728"/>
+        <c:crossAx val="-1459349776"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3340,7 +3392,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.0480821332366349"/>
           <c:y val="0.916768751571901"/>
-          <c:w val="0.9"/>
+          <c:w val="0.89810531496063"/>
           <c:h val="0.0523235117723307"/>
         </c:manualLayout>
       </c:layout>
@@ -5308,16 +5360,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5756,10 +5808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC40"/>
+  <dimension ref="A2:AJ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC2" workbookViewId="0">
-      <selection activeCell="AR27" sqref="AR27"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5772,7 +5824,7 @@
     <col min="21" max="22" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
@@ -5780,7 +5832,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>24</v>
@@ -5800,8 +5852,29 @@
       <c r="V2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>298.91699999999997</v>
       </c>
@@ -5834,40 +5907,48 @@
         <f>-H3</f>
         <v>-5604</v>
       </c>
+      <c r="T3" s="18">
+        <v>298.91699999999997</v>
+      </c>
       <c r="U3" s="37">
         <v>0.99638999999999989</v>
       </c>
       <c r="V3" s="37">
-        <v>-5.2321439999999999</v>
+        <f>D3*-1</f>
+        <v>5.2321439999999999</v>
       </c>
       <c r="W3">
-        <f>(V3-(0.2121*U3^5+0.0318*U3^4-0.1038*U3^3-0.0135*U3^2-5.3544*U3-0.0234))/V3*100</f>
+        <f>(V3+(0.2121*U3^5+0.0318*U3^4-0.1038*U3^3-0.0135*U3^2-5.3544*U3-0.0234))/V3*100</f>
         <v>-5.288073532217076E-2</v>
       </c>
       <c r="X3" s="2">
-        <f>(V3+(-0.211868*U3^5-0.0449275*U3^4+0.103505*U3^3+0.0297273*U3^2+5.35443*U3+0.0196438))/V3*100</f>
+        <f>(V3-(-0.211868*U3^5-0.0449275*U3^4+0.103505*U3^3+0.0297273*U3^2+5.35443*U3+0.0196438))/V3*100</f>
         <v>-4.1052028401682393E-2</v>
       </c>
       <c r="Y3" s="2">
         <v>1</v>
       </c>
       <c r="Z3" s="2">
-        <f>AA3*-1</f>
-        <v>-5.216545</v>
+        <v>5.216545</v>
       </c>
       <c r="AA3" s="2">
-        <v>5.216545</v>
-      </c>
-      <c r="AB3">
-        <f>(Z3-(0.2121*Y3^5+0.0318*Y3^4-0.1038*Y3^3-0.0135*Y3^2-5.3544*Y3-0.0234))*100</f>
-        <v>3.465499999999988</v>
-      </c>
-      <c r="AC3" s="2">
+        <f>(Z3+(0.2121*Y3^5+0.0318*Y3^4-0.1038*Y3^3-0.0135*Y3^2-5.3544*Y3-0.0234))*100</f>
+        <v>-3.465499999999988</v>
+      </c>
+      <c r="AB3" s="2">
         <f>((0.2734*Y3^5+0.0516*Y3^4-0.163*Y3^3-0.1018*Y3^2-5.2999*Y3+0.023)-(0.2121*Y3^5+0.0318*Y3^4-0.1038*Y3^3-0.0135*Y3^2-5.3544*Y3-0.0234))/((0.2121*Y3^5+0.0318*Y3^4-0.1038*Y3^3-0.0135*Y3^2-5.3544*Y3-0.0234))*100</f>
         <v>-0.65699268738573147</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AC3" s="2">
+        <f>(Z3-(-2.0398*Y3^5+4.0052*Y3^4-2.8535*Y3^3+0.8362*Y3^2+5.2388*Y3+0.0291))/Z3*100</f>
+        <v>1.044752800943528E-2</v>
+      </c>
+      <c r="AD3" s="2">
+        <f>(Z3-(-0.5949*Y3^3+0.6183*Y3^2+5.1663*Y3+0.0326))/Z3*100</f>
+        <v>-0.11032206182443997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>249.05199999999999</v>
       </c>
@@ -5900,40 +5981,52 @@
         <f t="shared" ref="I4:I17" si="3">-H4</f>
         <v>-4760</v>
       </c>
+      <c r="T4" s="20">
+        <v>249.05199999999999</v>
+      </c>
       <c r="U4" s="37">
         <v>0.83017333333333332</v>
       </c>
       <c r="V4" s="37">
-        <v>-4.4466604571428583</v>
+        <f t="shared" ref="V4:V9" si="4">D4*-1</f>
+        <v>4.4466604571428583</v>
       </c>
       <c r="W4" s="2">
-        <f>(V4-(0.212148*U4^5+0.031782*U4^4-0.103768*U4^3-0.013512*U4^2-5.354438*U4-0.023442))/V4*100</f>
-        <v>0.18380527272378616</v>
+        <f t="shared" ref="W4:W16" si="5">(V4+(0.2121*U4^5+0.0318*U4^4-0.1038*U4^3-0.0135*U4^2-5.3544*U4-0.0234))/V4*100</f>
+        <v>0.1850001172722297</v>
       </c>
       <c r="X4" s="2">
-        <f>(V4+(-0.211868*U4^5-0.0449275*U4^4+0.103505*U4^3+0.0297273*U4^2+5.35443*U4+0.0196438))/V4*100</f>
+        <f t="shared" ref="X4:X16" si="6">(V4-(-0.211868*U4^5-0.0449275*U4^4+0.103505*U4^3+0.0297273*U4^2+5.35443*U4+0.0196438))/V4*100</f>
         <v>0.1593682262741741</v>
       </c>
       <c r="Y4" s="2">
         <v>0.9</v>
       </c>
       <c r="Z4" s="2">
-        <f t="shared" ref="Z4:Z23" si="4">AA4*-1</f>
-        <v>-4.7529379999999994</v>
+        <v>4.7529379999999994</v>
       </c>
       <c r="AA4" s="2">
-        <v>4.7529379999999994</v>
+        <f t="shared" ref="AA4:AA23" si="7">(Z4+(0.2121*Y4^5+0.0318*Y4^4-0.1038*Y4^3-0.0135*Y4^2-5.3544*Y4-0.0234))*100</f>
+        <v>-2.9920291000000709</v>
       </c>
       <c r="AB4" s="2">
-        <f t="shared" ref="AB4:AB23" si="5">(Z4-(0.2121*Y4^5+0.0318*Y4^4-0.1038*Y4^3-0.0135*Y4^2-5.3544*Y4-0.0234))*100</f>
-        <v>2.9920291000000709</v>
+        <f t="shared" ref="AB4:AB23" si="8">((0.2734*Y4^5+0.0516*Y4^4-0.163*Y4^3-0.1018*Y4^2-5.2999*Y4+0.023)-(0.2121*Y4^5+0.0318*Y4^4-0.1038*Y4^3-0.0135*Y4^2-5.3544*Y4-0.0234))/((0.2121*Y4^5+0.0318*Y4^4-0.1038*Y4^3-0.0135*Y4^2-5.3544*Y4-0.0234))*100</f>
+        <v>-0.62636221224391986</v>
       </c>
       <c r="AC4" s="2">
-        <f t="shared" ref="AC4:AC23" si="6">((0.2734*Y4^5+0.0516*Y4^4-0.163*Y4^3-0.1018*Y4^2-5.2999*Y4+0.023)-(0.2121*Y4^5+0.0318*Y4^4-0.1038*Y4^3-0.0135*Y4^2-5.3544*Y4-0.0234))/((0.2121*Y4^5+0.0318*Y4^4-0.1038*Y4^3-0.0135*Y4^2-5.3544*Y4-0.0234))*100</f>
-        <v>-0.62636221224391986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AC4:AC12" si="9">(Z4-(-2.0398*Y4^5+4.0052*Y4^4-2.8535*Y4^3+0.8362*Y4^2+5.2388*Y4+0.0291))/Z4*100</f>
+        <v>-0.2426439814700016</v>
+      </c>
+      <c r="AD4" s="2">
+        <f t="shared" ref="AD4:AD12" si="10">(Z4-(-0.5949*Y4^3+0.6183*Y4^2+5.1663*Y4+0.0326))/Z4*100</f>
+        <v>7.4208836723715949E-2</v>
+      </c>
+      <c r="AJ4" t="e">
+        <f>(AG4-(-0.2734*AF4^5-0.0516*AF4^4+0.163*AF4^3+0.1018*AF4^2+5.2999*AF4-0.023))/AG4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>199.42599999999999</v>
       </c>
@@ -5966,40 +6059,48 @@
         <f t="shared" si="3"/>
         <v>-3827.5</v>
       </c>
+      <c r="T5" s="20">
+        <v>199.42599999999999</v>
+      </c>
       <c r="U5" s="37">
         <v>0.66475333333333331</v>
       </c>
       <c r="V5" s="37">
-        <v>-3.5810726285714285</v>
+        <f t="shared" si="4"/>
+        <v>3.5810726285714285</v>
       </c>
       <c r="W5" s="2">
-        <f>(V5-(0.212148*U5^5+0.031782*U5^4-0.103768*U5^3-0.013512*U5^2-5.354438*U5-0.023442))/V5*100</f>
-        <v>-0.12449218325171314</v>
+        <f t="shared" si="5"/>
+        <v>-0.12280421348984773</v>
       </c>
       <c r="X5" s="2">
-        <f>(V5+(-0.211868*U5^5-0.0449275*U5^4+0.103505*U5^3+0.0297273*U5^2+5.35443*U5+0.0196438))/V5*100</f>
+        <f t="shared" si="6"/>
         <v>-0.14555020695309168</v>
       </c>
       <c r="Y5" s="2">
         <v>0.8</v>
       </c>
       <c r="Z5" s="2">
-        <f t="shared" si="4"/>
-        <v>-4.2581040000000003</v>
+        <v>4.2581040000000003</v>
       </c>
       <c r="AA5" s="2">
-        <v>4.2581040000000003</v>
+        <f t="shared" si="7"/>
+        <v>-2.8075391999999866</v>
       </c>
       <c r="AB5" s="2">
-        <f t="shared" si="5"/>
-        <v>2.8075391999999866</v>
+        <f t="shared" si="8"/>
+        <v>-0.73199138744773673</v>
       </c>
       <c r="AC5" s="2">
-        <f t="shared" si="6"/>
-        <v>-0.73199138744773673</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-0.1958678322558452</v>
+      </c>
+      <c r="AD5" s="2">
+        <f t="shared" si="10"/>
+        <v>3.1488192867047765E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>149.70099999999999</v>
       </c>
@@ -6032,40 +6133,48 @@
         <f t="shared" si="3"/>
         <v>-2877</v>
       </c>
+      <c r="T6" s="20">
+        <v>149.70099999999999</v>
+      </c>
       <c r="U6" s="37">
         <v>0.4990033333333333</v>
       </c>
       <c r="V6" s="37">
-        <v>-2.6986378285714285</v>
+        <f t="shared" si="4"/>
+        <v>2.6986378285714285</v>
       </c>
       <c r="W6" s="2">
-        <f>(V6-(0.212148*U6^5+0.031782*U6^4-0.103768*U6^3-0.013512*U6^2-5.354438*U6-0.023442))/V6*100</f>
-        <v>-0.16342760070040951</v>
+        <f t="shared" si="5"/>
+        <v>-0.1612188938628327</v>
       </c>
       <c r="X6" s="2">
-        <f>(V6+(-0.211868*U6^5-0.0449275*U6^4+0.103505*U6^3+0.0297273*U6^2+5.35443*U6+0.0196438))/V6*100</f>
+        <f t="shared" si="6"/>
         <v>-0.14106112037716784</v>
       </c>
       <c r="Y6" s="2">
         <v>0.7</v>
       </c>
       <c r="Z6" s="2">
-        <f t="shared" si="4"/>
-        <v>-3.7322109999999999</v>
+        <v>3.7322109999999999</v>
       </c>
       <c r="AA6" s="2">
-        <v>3.7322109999999999</v>
+        <f t="shared" si="7"/>
+        <v>-3.8204572999999797</v>
       </c>
       <c r="AB6" s="2">
-        <f t="shared" si="5"/>
-        <v>3.8204572999999797</v>
+        <f t="shared" si="8"/>
+        <v>-0.95570555293799719</v>
       </c>
       <c r="AC6" s="2">
-        <f t="shared" si="6"/>
-        <v>-0.95570555293799719</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-0.37125001775087535</v>
+      </c>
+      <c r="AD6" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.42107212052050791</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>100.01900000000001</v>
       </c>
@@ -6098,40 +6207,48 @@
         <f t="shared" si="3"/>
         <v>-1928.5</v>
       </c>
+      <c r="T7" s="20">
+        <v>100.01900000000001</v>
+      </c>
       <c r="U7" s="37">
         <v>0.33339666666666667</v>
       </c>
       <c r="V7" s="37">
-        <v>-1.8137900857142857</v>
+        <f t="shared" si="4"/>
+        <v>1.8137900857142857</v>
       </c>
       <c r="W7" s="2">
-        <f>(V7-(0.212148*U7^5+0.031782*U7^4-0.103768*U7^3-0.013512*U7^2-5.354438*U7-0.023442))/V7*100</f>
-        <v>6.150027043097165E-2</v>
+        <f t="shared" si="5"/>
+        <v>6.4523868669465509E-2</v>
       </c>
       <c r="X7" s="2">
-        <f>(V7+(-0.211868*U7^5-0.0449275*U7^4+0.103505*U7^3+0.0297273*U7^2+5.35443*U7+0.0196438))/V7*100</f>
+        <f t="shared" si="6"/>
         <v>0.18111107402193619</v>
       </c>
       <c r="Y7" s="2">
         <v>0.6</v>
       </c>
       <c r="Z7" s="2">
-        <f t="shared" si="4"/>
-        <v>-3.1955339999999999</v>
+        <v>3.1955339999999999</v>
       </c>
       <c r="AA7" s="2">
-        <v>3.1955339999999999</v>
+        <f t="shared" si="7"/>
+        <v>-4.7172624000000329</v>
       </c>
       <c r="AB7" s="2">
-        <f t="shared" si="5"/>
-        <v>4.7172624000000329</v>
+        <f t="shared" si="8"/>
+        <v>-1.2908219229640867</v>
       </c>
       <c r="AC7" s="2">
-        <f t="shared" si="6"/>
-        <v>-1.2908219229640867</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-0.68786850648437592</v>
+      </c>
+      <c r="AD7" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.96808858863649694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>50.253999999999998</v>
       </c>
@@ -6164,40 +6281,48 @@
         <f t="shared" si="3"/>
         <v>-979</v>
       </c>
+      <c r="T8" s="20">
+        <v>50.253999999999998</v>
+      </c>
       <c r="U8" s="37">
         <v>0.16751333333333332</v>
       </c>
       <c r="V8" s="37">
-        <v>-0.92369939999999984</v>
+        <f t="shared" si="4"/>
+        <v>0.92369939999999984</v>
       </c>
       <c r="W8" s="2">
-        <f>(V8-(0.212148*U8^5+0.031782*U8^4-0.103768*U8^3-0.013512*U8^2-5.354438*U8-0.023442))/V8*100</f>
-        <v>0.27105438639858409</v>
+        <f t="shared" si="5"/>
+        <v>0.27631147110516124</v>
       </c>
       <c r="X8" s="2">
-        <f>(V8+(-0.211868*U8^5-0.0449275*U8^4+0.103505*U8^3+0.0297273*U8^2+5.35443*U8+0.0196438))/V8*100</f>
+        <f t="shared" si="6"/>
         <v>0.6343844148486355</v>
       </c>
       <c r="Y8" s="2">
         <v>0.5</v>
       </c>
       <c r="Z8" s="2">
-        <f t="shared" si="4"/>
-        <v>-2.6595</v>
+        <v>2.6595</v>
       </c>
       <c r="AA8" s="2">
-        <v>2.6595</v>
+        <f t="shared" si="7"/>
+        <v>-4.8834375000000207</v>
       </c>
       <c r="AB8" s="2">
-        <f t="shared" si="5"/>
-        <v>4.8834375000000207</v>
+        <f t="shared" si="8"/>
+        <v>-1.7474993278848878</v>
       </c>
       <c r="AC8" s="2">
-        <f t="shared" si="6"/>
-        <v>-1.7474993278848878</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-1.0507144200037744</v>
+      </c>
+      <c r="AD8" s="2">
+        <f t="shared" si="10"/>
+        <v>-1.3710283887948804</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>10.465999999999999</v>
       </c>
@@ -6230,40 +6355,48 @@
         <f t="shared" si="3"/>
         <v>-221</v>
       </c>
+      <c r="T9" s="20">
+        <v>10.465999999999999</v>
+      </c>
       <c r="U9" s="37">
         <v>3.4886666666666663E-2</v>
       </c>
       <c r="V9" s="37">
-        <v>-0.21197911428571428</v>
+        <f t="shared" si="4"/>
+        <v>0.21197911428571428</v>
       </c>
       <c r="W9" s="2">
-        <f>(V9-(0.212148*U9^5+0.031782*U9^4-0.103768*U9^3-0.013512*U9^2-5.354438*U9-0.023442))/V9*100</f>
-        <v>0.81037581824311289</v>
+        <f t="shared" si="5"/>
+        <v>0.83082073985766713</v>
       </c>
       <c r="X9" s="2">
-        <f>(V9+(-0.211868*U9^5-0.0449275*U9^4+0.103505*U9^3+0.0297273*U9^2+5.35443*U9+0.0196438))/V9*100</f>
+        <f t="shared" si="6"/>
         <v>2.592992195964869</v>
       </c>
       <c r="Y9" s="2">
         <v>0.4</v>
       </c>
       <c r="Z9" s="2">
-        <f t="shared" si="4"/>
-        <v>-2.1228029999999998</v>
+        <v>2.1228029999999998</v>
       </c>
       <c r="AA9" s="2">
-        <v>2.1228029999999998</v>
+        <f t="shared" si="7"/>
+        <v>-4.8174216000000492</v>
       </c>
       <c r="AB9" s="2">
-        <f t="shared" si="5"/>
-        <v>4.8174216000000492</v>
+        <f t="shared" si="8"/>
+        <v>-2.3684169332157592</v>
       </c>
       <c r="AC9" s="2">
-        <f t="shared" si="6"/>
-        <v>-2.3684169332157592</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-1.6313604229879226</v>
+      </c>
+      <c r="AD9" s="2">
+        <f t="shared" si="10"/>
+        <v>-1.7510527354634664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="27">
         <v>0</v>
@@ -6288,36 +6421,41 @@
         <v>-3.4966666666666667E-2</v>
       </c>
       <c r="V10" s="37">
-        <v>0.16482917142857145</v>
+        <f>D11*-1</f>
+        <v>-0.16482917142857145</v>
       </c>
       <c r="W10" s="2">
-        <f>(V10-(0.212148*U10^5+0.031782*U10^4-0.103768*U10^3-0.013512*U10^2-5.354438*U10-0.023442))/V10*100</f>
-        <v>0.64088813745165762</v>
+        <f t="shared" si="5"/>
+        <v>0.6162035893048553</v>
       </c>
       <c r="X10" s="2">
-        <f>(V10+(-0.211868*U10^5-0.0449275*U10^4+0.103505*U10^3+0.0297273*U10^2+5.35443*U10+0.0196438))/V10*100</f>
+        <f t="shared" si="6"/>
         <v>-1.6512442146239643</v>
       </c>
       <c r="Y10" s="2">
         <v>0.3</v>
       </c>
       <c r="Z10" s="2">
-        <f t="shared" si="4"/>
-        <v>-1.5847560000000001</v>
+        <v>1.5847560000000001</v>
       </c>
       <c r="AA10" s="2">
-        <v>1.5847560000000001</v>
+        <f t="shared" si="7"/>
+        <v>-4.8208617000000009</v>
       </c>
       <c r="AB10" s="2">
-        <f t="shared" si="5"/>
-        <v>4.8208617000000009</v>
+        <f t="shared" si="8"/>
+        <v>-3.2771034009489575</v>
       </c>
       <c r="AC10" s="2">
-        <f t="shared" si="6"/>
-        <v>-3.2771034009489575</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-2.6302412484950306</v>
+      </c>
+      <c r="AD10" s="2">
+        <f t="shared" si="10"/>
+        <v>-2.3548546274631366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>-10.49</v>
       </c>
@@ -6354,36 +6492,41 @@
         <v>-0.16777333333333333</v>
       </c>
       <c r="V11" s="37">
-        <v>0.8755328</v>
+        <f t="shared" ref="V11:V16" si="11">D12*-1</f>
+        <v>-0.8755328</v>
       </c>
       <c r="W11" s="2">
-        <f>(V11-(0.212148*U11^5+0.031782*U11^4-0.103768*U11^3-0.013512*U11^2-5.354438*U11-0.023442))/V11*100</f>
-        <v>6.1242869286582735E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.7115765320465396E-2</v>
       </c>
       <c r="X11" s="2">
-        <f>(V11+(-0.211868*U11^5-0.0449275*U11^4+0.103505*U11^3+0.0297273*U11^2+5.35443*U11+0.0196438))/V11*100</f>
+        <f t="shared" si="6"/>
         <v>-0.32134037042482072</v>
       </c>
       <c r="Y11" s="2">
         <v>0.2</v>
       </c>
       <c r="Z11" s="2">
-        <f t="shared" si="4"/>
-        <v>-1.0465629999999999</v>
+        <v>1.0465629999999999</v>
       </c>
       <c r="AA11" s="2">
-        <v>1.0465629999999999</v>
+        <f t="shared" si="7"/>
+        <v>-4.8968648000000226</v>
       </c>
       <c r="AB11" s="2">
-        <f t="shared" si="5"/>
-        <v>4.8968648000000226</v>
+        <f t="shared" si="8"/>
+        <v>-4.8693888576735871</v>
       </c>
       <c r="AC11" s="2">
-        <f t="shared" si="6"/>
-        <v>-4.8693888576735871</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-4.4596057762408918</v>
+      </c>
+      <c r="AD11" s="2">
+        <f t="shared" si="10"/>
+        <v>-3.7522633611163423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>-50.332000000000001</v>
       </c>
@@ -6420,36 +6563,41 @@
         <v>-0.33368666666666663</v>
       </c>
       <c r="V12" s="37">
-        <v>1.7643041428571429</v>
+        <f t="shared" si="11"/>
+        <v>-1.7643041428571429</v>
       </c>
       <c r="W12" s="2">
-        <f>(V12-(0.212148*U12^5+0.031782*U12^4-0.103768*U12^3-0.013512*U12^2-5.354438*U12-0.023442))/V12*100</f>
-        <v>-4.6803941962522314E-2</v>
+        <f t="shared" si="5"/>
+        <v>-4.8632808731838319E-2</v>
       </c>
       <c r="X12" s="2">
-        <f>(V12+(-0.211868*U12^5-0.0449275*U12^4+0.103505*U12^3+0.0297273*U12^2+5.35443*U12+0.0196438))/V12*100</f>
+        <f t="shared" si="6"/>
         <v>-0.16834618566214737</v>
       </c>
       <c r="Y12" s="2">
         <v>0.1</v>
       </c>
       <c r="Z12" s="2">
-        <f t="shared" si="4"/>
-        <v>-0.50851299999999999</v>
+        <v>0.50851299999999999</v>
       </c>
       <c r="AA12" s="2">
-        <v>0.50851299999999999</v>
+        <f t="shared" si="7"/>
+        <v>-5.0560499000000032</v>
       </c>
       <c r="AB12" s="2">
-        <f t="shared" si="5"/>
-        <v>5.0560499000000032</v>
+        <f t="shared" si="8"/>
+        <v>-9.1062075185216376</v>
       </c>
       <c r="AC12" s="2">
-        <f t="shared" si="6"/>
-        <v>-9.1062075185216376</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>-9.9025240259344383</v>
+      </c>
+      <c r="AD12" s="2">
+        <f t="shared" si="10"/>
+        <v>-9.1059815579935997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>-100.10599999999999</v>
       </c>
@@ -6486,33 +6634,31 @@
         <v>-0.49892666666666668</v>
       </c>
       <c r="V13" s="37">
-        <v>2.6480625714285715</v>
+        <f t="shared" si="11"/>
+        <v>-2.6480625714285715</v>
       </c>
       <c r="W13" s="2">
-        <f>(V13-(0.212148*U13^5+0.031782*U13^4-0.103768*U13^3-0.013512*U13^2-5.354438*U13-0.023442))/V13*100</f>
-        <v>-0.18511898959655171</v>
+        <f t="shared" si="5"/>
+        <v>-0.18635013708290543</v>
       </c>
       <c r="X13" s="2">
-        <f>(V13+(-0.211868*U13^5-0.0449275*U13^4+0.103505*U13^3+0.0297273*U13^2+5.35443*U13+0.0196438))/V13*100</f>
+        <f t="shared" si="6"/>
         <v>-0.20582559081158222</v>
       </c>
       <c r="Y13" s="2">
         <v>0</v>
       </c>
       <c r="Z13" s="2">
-        <f t="shared" si="4"/>
-        <v>2.9000000000000001E-2</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
       <c r="AA13" s="2">
-        <v>-2.9000000000000001E-2</v>
-      </c>
-      <c r="AB13" s="2">
-        <f t="shared" si="5"/>
-        <v>5.24</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>-5.24</v>
+      </c>
+      <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>-149.678</v>
       </c>
@@ -6549,36 +6695,34 @@
         <v>-0.66002000000000005</v>
       </c>
       <c r="V14" s="37">
-        <v>3.5298655714285712</v>
+        <f t="shared" si="11"/>
+        <v>-3.5298655714285712</v>
       </c>
       <c r="W14" s="2">
-        <f>(V14-(0.212148*U14^5+0.031782*U14^4-0.103768*U14^3-0.013512*U14^2-5.354438*U14-0.023442))/V14*100</f>
-        <v>0.44938591581374365</v>
+        <f t="shared" si="5"/>
+        <v>0.44823076024032049</v>
       </c>
       <c r="X14" s="2">
-        <f>(V14+(-0.211868*U14^5-0.0449275*U14^4+0.103505*U14^3+0.0297273*U14^2+5.35443*U14+0.0196438))/V14*100</f>
+        <f t="shared" si="6"/>
         <v>0.47252601374553244</v>
       </c>
       <c r="Y14" s="2">
         <v>-0.1</v>
       </c>
       <c r="Z14" s="2">
-        <f t="shared" si="4"/>
-        <v>0.55732999999999999</v>
+        <v>-0.55732999999999999</v>
       </c>
       <c r="AA14" s="2">
-        <v>-0.55732999999999999</v>
+        <f t="shared" si="7"/>
+        <v>-4.5320140999999925</v>
       </c>
       <c r="AB14" s="2">
-        <f t="shared" si="5"/>
-        <v>4.5320140999999925</v>
-      </c>
-      <c r="AC14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.8372645164240806</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AC14" s="2"/>
+    </row>
+    <row r="15" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>-198.006</v>
       </c>
@@ -6615,36 +6759,34 @@
         <v>-0.83118999999999998</v>
       </c>
       <c r="V15" s="37">
-        <v>4.3945141142857134</v>
+        <f t="shared" si="11"/>
+        <v>-4.3945141142857134</v>
       </c>
       <c r="W15" s="2">
-        <f>(V15-(0.212148*U15^5+0.031782*U15^4-0.103768*U15^3-0.013512*U15^2-5.354438*U15-0.023442))/V15*100</f>
-        <v>-0.31530214569691239</v>
+        <f t="shared" si="5"/>
+        <v>-0.31677480492965004</v>
       </c>
       <c r="X15" s="2">
-        <f>(V15+(-0.211868*U15^5-0.0449275*U15^4+0.103505*U15^3+0.0297273*U15^2+5.35443*U15+0.0196438))/V15*100</f>
+        <f t="shared" si="6"/>
         <v>-0.28852609737261548</v>
       </c>
       <c r="Y15" s="2">
         <v>-0.2</v>
       </c>
       <c r="Z15" s="2">
-        <f t="shared" si="4"/>
-        <v>1.081153</v>
+        <v>-1.081153</v>
       </c>
       <c r="AA15" s="2">
-        <v>-1.081153</v>
+        <f t="shared" si="7"/>
+        <v>-3.3399592000000089</v>
       </c>
       <c r="AB15" s="2">
-        <f t="shared" si="5"/>
-        <v>3.3399592000000089</v>
-      </c>
-      <c r="AC15" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.0974524875990821</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AC15" s="2"/>
+    </row>
+    <row r="16" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>-249.357</v>
       </c>
@@ -6681,34 +6823,32 @@
         <v>-0.99641000000000002</v>
       </c>
       <c r="V16" s="37">
-        <v>5.2279436857142851</v>
+        <f t="shared" si="11"/>
+        <v>-5.2279436857142851</v>
       </c>
       <c r="W16" s="2">
-        <f>(V16-(0.212148*U16^5+0.031782*U16^4-0.103768*U16^3-0.013512*U16^2-5.354438*U16-0.023442))/V16*100</f>
-        <v>7.593760387281312E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.3783898899894687E-2</v>
       </c>
       <c r="X16" s="2">
-        <f>(V16+(-0.211868*U16^5-0.0449275*U16^4+0.103505*U16^3+0.0297273*U16^2+5.35443*U16+0.0196438))/V16*100</f>
+        <f t="shared" si="6"/>
         <v>6.3241931296206713E-2</v>
       </c>
       <c r="Y16" s="2">
         <v>-0.3</v>
       </c>
       <c r="Z16" s="2">
-        <f t="shared" si="4"/>
-        <v>1.607812</v>
+        <v>-1.607812</v>
       </c>
       <c r="AA16" s="2">
-        <v>-1.607812</v>
+        <f t="shared" si="7"/>
+        <v>-2.3562223000000104</v>
       </c>
       <c r="AB16" s="2">
-        <f t="shared" si="5"/>
-        <v>2.3562223000000104</v>
-      </c>
-      <c r="AC16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.4967855034137045</v>
       </c>
+      <c r="AC16" s="2"/>
     </row>
     <row r="17" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
@@ -6747,40 +6887,34 @@
         <v>-0.4</v>
       </c>
       <c r="Z17" s="2">
-        <f t="shared" si="4"/>
-        <v>2.134096</v>
+        <v>-2.134096</v>
       </c>
       <c r="AA17" s="2">
-        <v>-2.134096</v>
+        <f t="shared" si="7"/>
+        <v>-1.2610624000000126</v>
       </c>
       <c r="AB17" s="2">
-        <f t="shared" si="5"/>
-        <v>1.2610624000000126</v>
-      </c>
-      <c r="AC17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.66651263119528215</v>
       </c>
+      <c r="AC17" s="2"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Y18" s="2">
         <v>-0.5</v>
       </c>
       <c r="Z18" s="2">
-        <f t="shared" si="4"/>
-        <v>2.6595490000000002</v>
+        <v>-2.6595490000000002</v>
       </c>
       <c r="AA18" s="2">
-        <v>-2.6595490000000002</v>
+        <f t="shared" si="7"/>
+        <v>-7.8962500000034908E-2</v>
       </c>
       <c r="AB18" s="2">
-        <f t="shared" si="5"/>
-        <v>7.8962500000034908E-2</v>
-      </c>
-      <c r="AC18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.14280626655055487</v>
       </c>
+      <c r="AC18" s="2"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B19" s="24" t="s">
@@ -6802,20 +6936,17 @@
         <v>-0.6</v>
       </c>
       <c r="Z19" s="2">
-        <f t="shared" si="4"/>
-        <v>3.1828699999999999</v>
+        <v>-3.1828699999999999</v>
       </c>
       <c r="AA19" s="2">
-        <v>-3.1828699999999999</v>
+        <f t="shared" si="7"/>
+        <v>1.1559183999999778</v>
       </c>
       <c r="AB19" s="2">
-        <f t="shared" si="5"/>
-        <v>-1.1559183999999778</v>
-      </c>
-      <c r="AC19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.23482780703269285</v>
       </c>
+      <c r="AC19" s="2"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
@@ -6842,40 +6973,34 @@
         <v>-0.7</v>
       </c>
       <c r="Z20" s="2">
-        <f t="shared" si="4"/>
-        <v>3.7033260000000001</v>
+        <v>-3.7033260000000001</v>
       </c>
       <c r="AA20" s="2">
-        <v>-3.7033260000000001</v>
+        <f t="shared" si="7"/>
+        <v>2.2329932999999524</v>
       </c>
       <c r="AB20" s="2">
-        <f t="shared" si="5"/>
-        <v>-2.2329932999999524</v>
-      </c>
-      <c r="AC20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.54379983993007552</v>
       </c>
+      <c r="AC20" s="2"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Y21" s="2">
         <v>-0.8</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" si="4"/>
-        <v>4.2175739999999999</v>
+        <v>-4.2175739999999999</v>
       </c>
       <c r="AA21" s="2">
-        <v>-4.2175739999999999</v>
+        <f t="shared" si="7"/>
+        <v>3.0575952000000406</v>
       </c>
       <c r="AB21" s="2">
-        <f t="shared" si="5"/>
-        <v>-3.0575952000000406</v>
-      </c>
-      <c r="AC21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.83279320174053895</v>
       </c>
+      <c r="AC21" s="2"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -6885,20 +7010,17 @@
         <v>-0.9</v>
       </c>
       <c r="Z22" s="2">
-        <f t="shared" si="4"/>
-        <v>4.7064170000000001</v>
+        <v>-4.7064170000000001</v>
       </c>
       <c r="AA22" s="2">
-        <v>-4.7064170000000001</v>
+        <f t="shared" si="7"/>
+        <v>4.9499251000001188</v>
       </c>
       <c r="AB22" s="2">
-        <f t="shared" si="5"/>
-        <v>-4.9499251000001188</v>
-      </c>
-      <c r="AC22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.1401053790339672</v>
       </c>
+      <c r="AC22" s="2"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
@@ -6908,20 +7030,17 @@
         <v>-1</v>
       </c>
       <c r="Z23" s="2">
-        <f t="shared" si="4"/>
-        <v>5.1583769999999998</v>
+        <v>-5.1583769999999998</v>
       </c>
       <c r="AA23" s="2">
-        <v>-5.1583769999999998</v>
+        <f t="shared" si="7"/>
+        <v>8.2623000000000779</v>
       </c>
       <c r="AB23" s="2">
-        <f t="shared" si="5"/>
-        <v>-8.2623000000000779</v>
-      </c>
-      <c r="AC23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-1.5016218278954478</v>
       </c>
+      <c r="AC23" s="2"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
@@ -6966,11 +7085,11 @@
         <v>249.05199999999999</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" ref="M27:M40" si="7">L27/300</f>
+        <f t="shared" ref="M27:M40" si="12">L27/300</f>
         <v>0.83017333333333332</v>
       </c>
       <c r="N27" s="34">
-        <f t="shared" ref="N27:N40" si="8">O27/10000</f>
+        <f t="shared" ref="N27:N40" si="13">O27/10000</f>
         <v>-4.4466604571428583</v>
       </c>
       <c r="O27" s="21">
@@ -6992,11 +7111,11 @@
         <v>199.42599999999999</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.66475333333333331</v>
       </c>
       <c r="N28" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-3.5810726285714285</v>
       </c>
       <c r="O28" s="21">
@@ -7011,11 +7130,11 @@
         <v>149.70099999999999</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.4990033333333333</v>
       </c>
       <c r="N29" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-2.6986378285714285</v>
       </c>
       <c r="O29" s="21">
@@ -7030,11 +7149,11 @@
         <v>100.01900000000001</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.33339666666666667</v>
       </c>
       <c r="N30" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-1.8137900857142857</v>
       </c>
       <c r="O30" s="21">
@@ -7049,11 +7168,11 @@
         <v>50.253999999999998</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.16751333333333332</v>
       </c>
       <c r="N31" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-0.92369939999999984</v>
       </c>
       <c r="O31" s="21">
@@ -7068,11 +7187,11 @@
         <v>10.465999999999999</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3.4886666666666663E-2</v>
       </c>
       <c r="N32" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>-0.21197911428571428</v>
       </c>
       <c r="O32" s="21">
@@ -7085,11 +7204,11 @@
       </c>
       <c r="L33" s="20"/>
       <c r="M33" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N33" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O33" s="21"/>
@@ -7102,11 +7221,11 @@
         <v>-10.49</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-3.4966666666666667E-2</v>
       </c>
       <c r="N34" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.16482917142857145</v>
       </c>
       <c r="O34" s="21">
@@ -7121,11 +7240,11 @@
         <v>-50.332000000000001</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-0.16777333333333333</v>
       </c>
       <c r="N35" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.8755328</v>
       </c>
       <c r="O35" s="21">
@@ -7140,11 +7259,11 @@
         <v>-100.10599999999999</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-0.33368666666666663</v>
       </c>
       <c r="N36" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1.7643041428571429</v>
       </c>
       <c r="O36" s="21">
@@ -7159,11 +7278,11 @@
         <v>-149.678</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-0.49892666666666668</v>
       </c>
       <c r="N37" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>2.6480625714285715</v>
       </c>
       <c r="O37" s="21">
@@ -7178,11 +7297,11 @@
         <v>-198.006</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-0.66002000000000005</v>
       </c>
       <c r="N38" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3.5298655714285712</v>
       </c>
       <c r="O38" s="21">
@@ -7197,11 +7316,11 @@
         <v>-249.357</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-0.83118999999999998</v>
       </c>
       <c r="N39" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>4.3945141142857134</v>
       </c>
       <c r="O39" s="21">
@@ -7216,11 +7335,11 @@
         <v>-298.923</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-0.99641000000000002</v>
       </c>
       <c r="N40" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>5.2279436857142851</v>
       </c>
       <c r="O40" s="23">
@@ -7228,6 +7347,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="Z3:Z23">
+    <sortCondition ref="Z3"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B26:C26"/>
   </mergeCells>
@@ -7246,7 +7368,7 @@
   <dimension ref="B1:M106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edits to NIM and quad technote and MollerRunsDB
</commit_message>
<xml_diff>
--- a/quads/Patsy2012.xlsx
+++ b/quads/Patsy2012.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1540" windowWidth="26920" windowHeight="16260"/>
+    <workbookView xWindow="1880" yWindow="680" windowWidth="26920" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>BL</t>
   </si>
@@ -41,10 +41,6 @@
   <si>
     <t>Transducer Readback
 Current (A)</t>
-  </si>
-  <si>
-    <t>Measured
-GL (G)</t>
   </si>
   <si>
     <t>Set Current
@@ -379,7 +375,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,15 +446,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -470,6 +457,18 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -648,8 +647,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1607198592"/>
-        <c:axId val="-1607195888"/>
+        <c:axId val="1281589392"/>
+        <c:axId val="1281591712"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -790,11 +789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1607190608"/>
-        <c:axId val="-1607193328"/>
+        <c:axId val="1279689584"/>
+        <c:axId val="1281594032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1607198592"/>
+        <c:axId val="1281589392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,12 +803,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-1607195888"/>
+        <c:crossAx val="1281591712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1607195888"/>
+        <c:axId val="1281591712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000.0"/>
@@ -822,12 +821,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="-1607198592"/>
+        <c:crossAx val="1281589392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1607193328"/>
+        <c:axId val="1281594032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,12 +836,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1607190608"/>
+        <c:crossAx val="1279689584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1607190608"/>
+        <c:axId val="1279689584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-1607193328"/>
+        <c:crossAx val="1281594032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -983,7 +982,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Measured_x000d_GL (G)</c:v>
+                  <c:v>Measured_x000d_GL (T)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1174,8 +1173,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1523489008"/>
-        <c:axId val="-1495687312"/>
+        <c:axId val="1280119504"/>
+        <c:axId val="1280122624"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1468,11 +1467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1477623968"/>
-        <c:axId val="-1526684528"/>
+        <c:axId val="1252411968"/>
+        <c:axId val="1280126928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1523489008"/>
+        <c:axId val="1280119504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1589,13 +1588,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1495687312"/>
+        <c:crossAx val="1280122624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1495687312"/>
+        <c:axId val="1280122624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,12 +1716,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1523489008"/>
+        <c:crossAx val="1280119504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1526684528"/>
+        <c:axId val="1280126928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -1837,12 +1836,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1477623968"/>
+        <c:crossAx val="1252411968"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1477623968"/>
+        <c:axId val="1252411968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1851,7 +1850,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1526684528"/>
+        <c:crossAx val="1280126928"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2053,196 +2053,6 @@
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Difference x100 (T)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="00B0F0"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Summary!$Y$3:$Y$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-0.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-0.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-0.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-0.9</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Summary!$AA$3:$AA$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>-3.465499999999988</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.992029100000071</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.807539199999987</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-3.82045729999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-4.717262400000032</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-4.883437500000021</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.817421600000049</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4.820861700000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-4.896864800000022</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-5.056049900000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-5.24</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-4.532014099999992</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-3.339959200000009</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2.35622230000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.261062400000013</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-0.0789625000000349</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.155918399999978</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.232993299999952</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.057595200000041</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.949925100000118</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8.262300000000078</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-1493616000"/>
-        <c:axId val="-1526539328"/>
-      </c:scatterChart>
-      <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -2859,8 +2669,198 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1493616000"/>
-        <c:axId val="-1526539328"/>
+        <c:axId val="1281671568"/>
+        <c:axId val="1281674000"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Difference x100 (T)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Summary!$Y$3:$Y$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Summary!$AA$3:$AA$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-3.465499999999988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.992029100000071</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.807539199999987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.82045729999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.717262400000032</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.883437500000021</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.817421600000049</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.820861700000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4.896864800000022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.056049900000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.532014099999992</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.339959200000009</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.35622230000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.261062400000013</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.0789625000000349</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.155918399999978</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.232993299999952</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.057595200000041</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.949925100000118</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.262300000000078</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1281671568"/>
+        <c:axId val="1281674000"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -3046,11 +3046,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1630977712"/>
-        <c:axId val="-1459349776"/>
+        <c:axId val="1281680224"/>
+        <c:axId val="1281677392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1493616000"/>
+        <c:axId val="1281671568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,12 +3168,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1526539328"/>
+        <c:crossAx val="1281674000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1526539328"/>
+        <c:axId val="1281674000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0"/>
@@ -3301,13 +3301,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1493616000"/>
+        <c:crossAx val="1281671568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1459349776"/>
+        <c:axId val="1281677392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12.0"/>
@@ -3350,13 +3350,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1630977712"/>
+        <c:crossAx val="1281680224"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1630977712"/>
+        <c:axId val="1281680224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3365,7 +3365,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1459349776"/>
+        <c:crossAx val="1281677392"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4137,11 +4138,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1607163008"/>
-        <c:axId val="-1606898608"/>
+        <c:axId val="1281704464"/>
+        <c:axId val="1281706784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1607163008"/>
+        <c:axId val="1281704464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4151,12 +4152,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1606898608"/>
+        <c:crossAx val="1281706784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1606898608"/>
+        <c:axId val="1281706784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1607163008"/>
+        <c:crossAx val="1281704464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5810,8 +5811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="R18" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3:V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5821,57 +5822,58 @@
     <col min="4" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="21" max="22" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:36" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="U2" t="s">
         <v>2</v>
       </c>
-      <c r="V2" t="s">
-        <v>3</v>
+      <c r="V2" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" t="s">
         <v>25</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" t="s">
-        <v>30</v>
-      </c>
       <c r="AC2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5885,7 +5887,7 @@
         <f>A3/300</f>
         <v>0.99638999999999989</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="30">
         <f>G3/10000</f>
         <v>-5.2321439999999999</v>
       </c>
@@ -5910,10 +5912,10 @@
       <c r="T3" s="18">
         <v>298.91699999999997</v>
       </c>
-      <c r="U3" s="37">
+      <c r="U3" s="34">
         <v>0.99638999999999989</v>
       </c>
-      <c r="V3" s="37">
+      <c r="V3" s="34">
         <f>D3*-1</f>
         <v>5.2321439999999999</v>
       </c>
@@ -5959,7 +5961,7 @@
         <f t="shared" ref="C4:C17" si="0">A4/300</f>
         <v>0.83017333333333332</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="30">
         <f t="shared" ref="D4:D17" si="1">G4/10000</f>
         <v>-4.4466604571428583</v>
       </c>
@@ -5984,10 +5986,10 @@
       <c r="T4" s="20">
         <v>249.05199999999999</v>
       </c>
-      <c r="U4" s="37">
+      <c r="U4" s="34">
         <v>0.83017333333333332</v>
       </c>
-      <c r="V4" s="37">
+      <c r="V4" s="34">
         <f t="shared" ref="V4:V9" si="4">D4*-1</f>
         <v>4.4466604571428583</v>
       </c>
@@ -6037,7 +6039,7 @@
         <f t="shared" si="0"/>
         <v>0.66475333333333331</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="30">
         <f t="shared" si="1"/>
         <v>-3.5810726285714285</v>
       </c>
@@ -6062,10 +6064,10 @@
       <c r="T5" s="20">
         <v>199.42599999999999</v>
       </c>
-      <c r="U5" s="37">
+      <c r="U5" s="34">
         <v>0.66475333333333331</v>
       </c>
-      <c r="V5" s="37">
+      <c r="V5" s="34">
         <f t="shared" si="4"/>
         <v>3.5810726285714285</v>
       </c>
@@ -6111,7 +6113,7 @@
         <f t="shared" si="0"/>
         <v>0.4990033333333333</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="30">
         <f t="shared" si="1"/>
         <v>-2.6986378285714285</v>
       </c>
@@ -6136,10 +6138,10 @@
       <c r="T6" s="20">
         <v>149.70099999999999</v>
       </c>
-      <c r="U6" s="37">
+      <c r="U6" s="34">
         <v>0.4990033333333333</v>
       </c>
-      <c r="V6" s="37">
+      <c r="V6" s="34">
         <f t="shared" si="4"/>
         <v>2.6986378285714285</v>
       </c>
@@ -6185,7 +6187,7 @@
         <f t="shared" si="0"/>
         <v>0.33339666666666667</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="30">
         <f t="shared" si="1"/>
         <v>-1.8137900857142857</v>
       </c>
@@ -6210,10 +6212,10 @@
       <c r="T7" s="20">
         <v>100.01900000000001</v>
       </c>
-      <c r="U7" s="37">
+      <c r="U7" s="34">
         <v>0.33339666666666667</v>
       </c>
-      <c r="V7" s="37">
+      <c r="V7" s="34">
         <f t="shared" si="4"/>
         <v>1.8137900857142857</v>
       </c>
@@ -6259,7 +6261,7 @@
         <f t="shared" si="0"/>
         <v>0.16751333333333332</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="30">
         <f t="shared" si="1"/>
         <v>-0.92369939999999984</v>
       </c>
@@ -6284,10 +6286,10 @@
       <c r="T8" s="20">
         <v>50.253999999999998</v>
       </c>
-      <c r="U8" s="37">
+      <c r="U8" s="34">
         <v>0.16751333333333332</v>
       </c>
-      <c r="V8" s="37">
+      <c r="V8" s="34">
         <f t="shared" si="4"/>
         <v>0.92369939999999984</v>
       </c>
@@ -6333,7 +6335,7 @@
         <f t="shared" si="0"/>
         <v>3.4886666666666663E-2</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="30">
         <f t="shared" si="1"/>
         <v>-0.21197911428571428</v>
       </c>
@@ -6358,10 +6360,10 @@
       <c r="T9" s="20">
         <v>10.465999999999999</v>
       </c>
-      <c r="U9" s="37">
+      <c r="U9" s="34">
         <v>3.4886666666666663E-2</v>
       </c>
-      <c r="V9" s="37">
+      <c r="V9" s="34">
         <f t="shared" si="4"/>
         <v>0.21197911428571428</v>
       </c>
@@ -6405,7 +6407,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="16"/>
       <c r="F10" s="7"/>
       <c r="G10" s="21"/>
@@ -6417,10 +6419,10 @@
         <f t="shared" si="3"/>
         <v>-24</v>
       </c>
-      <c r="U10" s="37">
+      <c r="U10" s="34">
         <v>-3.4966666666666667E-2</v>
       </c>
-      <c r="V10" s="37">
+      <c r="V10" s="34">
         <f>D11*-1</f>
         <v>-0.16482917142857145</v>
       </c>
@@ -6466,7 +6468,7 @@
         <f t="shared" si="0"/>
         <v>-3.4966666666666667E-2</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="30">
         <f t="shared" si="1"/>
         <v>0.16482917142857145</v>
       </c>
@@ -6488,10 +6490,10 @@
         <f t="shared" si="3"/>
         <v>174.5</v>
       </c>
-      <c r="U11" s="37">
+      <c r="U11" s="34">
         <v>-0.16777333333333333</v>
       </c>
-      <c r="V11" s="37">
+      <c r="V11" s="34">
         <f t="shared" ref="V11:V16" si="11">D12*-1</f>
         <v>-0.8755328</v>
       </c>
@@ -6537,7 +6539,7 @@
         <f t="shared" si="0"/>
         <v>-0.16777333333333333</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="30">
         <f t="shared" si="1"/>
         <v>0.8755328</v>
       </c>
@@ -6559,10 +6561,10 @@
         <f t="shared" si="3"/>
         <v>929.5</v>
       </c>
-      <c r="U12" s="37">
+      <c r="U12" s="34">
         <v>-0.33368666666666663</v>
       </c>
-      <c r="V12" s="37">
+      <c r="V12" s="34">
         <f t="shared" si="11"/>
         <v>-1.7643041428571429</v>
       </c>
@@ -6608,7 +6610,7 @@
         <f t="shared" si="0"/>
         <v>-0.33368666666666663</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="30">
         <f t="shared" si="1"/>
         <v>1.7643041428571429</v>
       </c>
@@ -6630,10 +6632,10 @@
         <f t="shared" si="3"/>
         <v>1872.5</v>
       </c>
-      <c r="U13" s="37">
+      <c r="U13" s="34">
         <v>-0.49892666666666668</v>
       </c>
-      <c r="V13" s="37">
+      <c r="V13" s="34">
         <f t="shared" si="11"/>
         <v>-2.6480625714285715</v>
       </c>
@@ -6669,7 +6671,7 @@
         <f t="shared" si="0"/>
         <v>-0.49892666666666668</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="30">
         <f t="shared" si="1"/>
         <v>2.6480625714285715</v>
       </c>
@@ -6691,10 +6693,10 @@
         <f t="shared" si="3"/>
         <v>2811</v>
       </c>
-      <c r="U14" s="37">
+      <c r="U14" s="34">
         <v>-0.66002000000000005</v>
       </c>
-      <c r="V14" s="37">
+      <c r="V14" s="34">
         <f t="shared" si="11"/>
         <v>-3.5298655714285712</v>
       </c>
@@ -6733,7 +6735,7 @@
         <f t="shared" si="0"/>
         <v>-0.66002000000000005</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="30">
         <f t="shared" si="1"/>
         <v>3.5298655714285712</v>
       </c>
@@ -6755,10 +6757,10 @@
         <f t="shared" si="3"/>
         <v>3749.5</v>
       </c>
-      <c r="U15" s="37">
+      <c r="U15" s="34">
         <v>-0.83118999999999998</v>
       </c>
-      <c r="V15" s="37">
+      <c r="V15" s="34">
         <f t="shared" si="11"/>
         <v>-4.3945141142857134</v>
       </c>
@@ -6797,7 +6799,7 @@
         <f t="shared" si="0"/>
         <v>-0.83118999999999998</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="30">
         <f t="shared" si="1"/>
         <v>4.3945141142857134</v>
       </c>
@@ -6819,10 +6821,10 @@
         <f t="shared" si="3"/>
         <v>4668.5</v>
       </c>
-      <c r="U16" s="37">
+      <c r="U16" s="34">
         <v>-0.99641000000000002</v>
       </c>
-      <c r="V16" s="37">
+      <c r="V16" s="34">
         <f t="shared" si="11"/>
         <v>-5.2279436857142851</v>
       </c>
@@ -6861,7 +6863,7 @@
         <f t="shared" si="0"/>
         <v>-0.99641000000000002</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="30">
         <f t="shared" si="1"/>
         <v>5.2279436857142851</v>
       </c>
@@ -6918,19 +6920,19 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B19" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y19" s="2">
         <v>-0.6</v>
@@ -7004,7 +7006,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y22" s="2">
         <v>-0.9</v>
@@ -7024,7 +7026,7 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y23" s="2">
         <v>-1</v>
@@ -7044,15 +7046,15 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="31"/>
+      <c r="B26" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="36"/>
       <c r="K26" s="14">
         <v>300</v>
       </c>
@@ -7063,7 +7065,7 @@
         <f>L26/300</f>
         <v>0.99638999999999989</v>
       </c>
-      <c r="N26" s="34">
+      <c r="N26" s="31">
         <f>O26/10000</f>
         <v>-5.2321439999999999</v>
       </c>
@@ -7073,7 +7075,7 @@
     </row>
     <row r="27" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3">
         <v>4</v>
@@ -7088,7 +7090,7 @@
         <f t="shared" ref="M27:M40" si="12">L27/300</f>
         <v>0.83017333333333332</v>
       </c>
-      <c r="N27" s="34">
+      <c r="N27" s="31">
         <f t="shared" ref="N27:N40" si="13">O27/10000</f>
         <v>-4.4466604571428583</v>
       </c>
@@ -7098,7 +7100,7 @@
     </row>
     <row r="28" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3">
         <f>4-0.065*2</f>
@@ -7114,7 +7116,7 @@
         <f t="shared" si="12"/>
         <v>0.66475333333333331</v>
       </c>
-      <c r="N28" s="34">
+      <c r="N28" s="31">
         <f t="shared" si="13"/>
         <v>-3.5810726285714285</v>
       </c>
@@ -7133,7 +7135,7 @@
         <f t="shared" si="12"/>
         <v>0.4990033333333333</v>
       </c>
-      <c r="N29" s="34">
+      <c r="N29" s="31">
         <f t="shared" si="13"/>
         <v>-2.6986378285714285</v>
       </c>
@@ -7152,7 +7154,7 @@
         <f t="shared" si="12"/>
         <v>0.33339666666666667</v>
       </c>
-      <c r="N30" s="34">
+      <c r="N30" s="31">
         <f t="shared" si="13"/>
         <v>-1.8137900857142857</v>
       </c>
@@ -7171,7 +7173,7 @@
         <f t="shared" si="12"/>
         <v>0.16751333333333332</v>
       </c>
-      <c r="N31" s="34">
+      <c r="N31" s="31">
         <f t="shared" si="13"/>
         <v>-0.92369939999999984</v>
       </c>
@@ -7190,7 +7192,7 @@
         <f t="shared" si="12"/>
         <v>3.4886666666666663E-2</v>
       </c>
-      <c r="N32" s="34">
+      <c r="N32" s="31">
         <f t="shared" si="13"/>
         <v>-0.21197911428571428</v>
       </c>
@@ -7207,7 +7209,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="N33" s="34">
+      <c r="N33" s="31">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7224,7 +7226,7 @@
         <f t="shared" si="12"/>
         <v>-3.4966666666666667E-2</v>
       </c>
-      <c r="N34" s="34">
+      <c r="N34" s="31">
         <f t="shared" si="13"/>
         <v>0.16482917142857145</v>
       </c>
@@ -7243,7 +7245,7 @@
         <f t="shared" si="12"/>
         <v>-0.16777333333333333</v>
       </c>
-      <c r="N35" s="34">
+      <c r="N35" s="31">
         <f t="shared" si="13"/>
         <v>0.8755328</v>
       </c>
@@ -7262,7 +7264,7 @@
         <f t="shared" si="12"/>
         <v>-0.33368666666666663</v>
       </c>
-      <c r="N36" s="34">
+      <c r="N36" s="31">
         <f t="shared" si="13"/>
         <v>1.7643041428571429</v>
       </c>
@@ -7281,7 +7283,7 @@
         <f t="shared" si="12"/>
         <v>-0.49892666666666668</v>
       </c>
-      <c r="N37" s="34">
+      <c r="N37" s="31">
         <f t="shared" si="13"/>
         <v>2.6480625714285715</v>
       </c>
@@ -7300,7 +7302,7 @@
         <f t="shared" si="12"/>
         <v>-0.66002000000000005</v>
       </c>
-      <c r="N38" s="34">
+      <c r="N38" s="31">
         <f t="shared" si="13"/>
         <v>3.5298655714285712</v>
       </c>
@@ -7319,7 +7321,7 @@
         <f t="shared" si="12"/>
         <v>-0.83118999999999998</v>
       </c>
-      <c r="N39" s="34">
+      <c r="N39" s="31">
         <f t="shared" si="13"/>
         <v>4.3945141142857134</v>
       </c>
@@ -7338,7 +7340,7 @@
         <f t="shared" si="12"/>
         <v>-0.99641000000000002</v>
       </c>
-      <c r="N40" s="34">
+      <c r="N40" s="31">
         <f t="shared" si="13"/>
         <v>5.2279436857142851</v>
       </c>
@@ -7384,24 +7386,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="E1" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="32"/>
-      <c r="I1" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="31"/>
+      <c r="E1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="37"/>
+      <c r="I1" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="3">
         <v>4</v>
@@ -7424,7 +7426,7 @@
         <v>5.7859625668449191</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" s="3">
         <f>4-0.065*2</f>
@@ -7448,19 +7450,19 @@
         <v>13.21042780748663</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="L4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
@@ -7486,7 +7488,7 @@
         <f>I5*50</f>
         <v>298.98500000000001</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="32">
         <f>SUMPRODUCT(F3:F106,E3:E106)</f>
         <v>253526.3767727474</v>
       </c>
@@ -7494,7 +7496,7 @@
         <f>F54</f>
         <v>-5668.3999999999987</v>
       </c>
-      <c r="M5" s="36">
+      <c r="M5" s="33">
         <f>ABS(K5/L5)</f>
         <v>44.726267866196359</v>
       </c>
@@ -7533,7 +7535,7 @@
         <v>20.37887700534759</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">

</xml_diff>